<commit_message>
changed acc5 and acc1 to report only for fine labels
</commit_message>
<xml_diff>
--- a/experiments/mac_multi/eval_19/classification_report_19.xlsx
+++ b/experiments/mac_multi/eval_19/classification_report_19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-mpg microgesture\human_micro_gesture_classifier\experiments\mac_multi\eval_19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DADD8AD4-E248-474F-BFB0-C62A8573DAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D810A18C-5AFA-4F68-95E6-9779E2D6F842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CD57265-B7E1-49FF-A597-D1A83EF28E7E}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="145">
   <si>
     <t>labels</t>
   </si>
@@ -58,12 +58,6 @@
     <t>0.39658848614072495</t>
   </si>
   <si>
-    <t>0.3691670184996065</t>
-  </si>
-  <si>
-    <t>0.9412889519265586</t>
-  </si>
-  <si>
     <t>sitting straightly</t>
   </si>
   <si>
@@ -76,24 +70,12 @@
     <t>0.22018348623853212</t>
   </si>
   <si>
-    <t>0.19249731191673541</t>
-  </si>
-  <si>
-    <t>0.9375232907072529</t>
-  </si>
-  <si>
     <t>shrugging</t>
   </si>
   <si>
-    <t>0.9000059769290538</t>
-  </si>
-  <si>
     <t>turning around</t>
   </si>
   <si>
-    <t>0.7435070750492567</t>
-  </si>
-  <si>
     <t>rising up</t>
   </si>
   <si>
@@ -103,39 +85,18 @@
     <t>0.42857142857142855</t>
   </si>
   <si>
-    <t>0.43162824274395717</t>
-  </si>
-  <si>
-    <t>0.9523330786130482</t>
-  </si>
-  <si>
     <t>bowing head</t>
   </si>
   <si>
-    <t>0.6744246471198299</t>
-  </si>
-  <si>
     <t>head up</t>
   </si>
   <si>
-    <t>0.7032914187201803</t>
-  </si>
-  <si>
     <t>tilting head</t>
   </si>
   <si>
-    <t>0.7106867579549845</t>
-  </si>
-  <si>
     <t>turning head</t>
   </si>
   <si>
-    <t>0.21718854985321673</t>
-  </si>
-  <si>
-    <t>0.7472399709492101</t>
-  </si>
-  <si>
     <t>nodding</t>
   </si>
   <si>
@@ -145,9 +106,6 @@
     <t>0.43943298969072164</t>
   </si>
   <si>
-    <t>0.35603561386511917</t>
-  </si>
-  <si>
     <t>shaking head</t>
   </si>
   <si>
@@ -157,12 +115,6 @@
     <t>0.2393162393162393</t>
   </si>
   <si>
-    <t>0.3590722140429383</t>
-  </si>
-  <si>
-    <t>0.8543554869353072</t>
-  </si>
-  <si>
     <t>scratching arms</t>
   </si>
   <si>
@@ -172,48 +124,21 @@
     <t>0.45535714285714285</t>
   </si>
   <si>
-    <t>0.3887437425440325</t>
-  </si>
-  <si>
-    <t>0.9444476160029229</t>
-  </si>
-  <si>
     <t>playing objects</t>
   </si>
   <si>
-    <t>0.041903223956590005</t>
-  </si>
-  <si>
-    <t>0.8136205114957376</t>
-  </si>
-  <si>
     <t>putting hands together</t>
   </si>
   <si>
-    <t>0.7873223909377605</t>
-  </si>
-  <si>
     <t>rubbing hands</t>
   </si>
   <si>
-    <t>0.9084071364394815</t>
-  </si>
-  <si>
     <t>pointing oneself</t>
   </si>
   <si>
-    <t>0.14274661161155783</t>
-  </si>
-  <si>
-    <t>0.9307000373881106</t>
-  </si>
-  <si>
     <t>clenching fist</t>
   </si>
   <si>
-    <t>0.8307194381261781</t>
-  </si>
-  <si>
     <t>stretching arms</t>
   </si>
   <si>
@@ -226,18 +151,9 @@
     <t>0.3116883116883117</t>
   </si>
   <si>
-    <t>0.22035539123452189</t>
-  </si>
-  <si>
-    <t>0.9259473197781886</t>
-  </si>
-  <si>
     <t>retracting arms</t>
   </si>
   <si>
-    <t>0.8889653407398395</t>
-  </si>
-  <si>
     <t>waving</t>
   </si>
   <si>
@@ -250,39 +166,18 @@
     <t>0.33183856502242154</t>
   </si>
   <si>
-    <t>0.32126225153539045</t>
-  </si>
-  <si>
-    <t>0.9415521451829152</t>
-  </si>
-  <si>
     <t>spreading hands</t>
   </si>
   <si>
-    <t>0.15414489762337355</t>
-  </si>
-  <si>
-    <t>0.9295376557029585</t>
-  </si>
-  <si>
     <t>hands touching fingers</t>
   </si>
   <si>
     <t>0.3333333333333333</t>
   </si>
   <si>
-    <t>0.20397310985488062</t>
-  </si>
-  <si>
-    <t>0.8622739042378627</t>
-  </si>
-  <si>
     <t>other finger movements</t>
   </si>
   <si>
-    <t>0.7908333333333333</t>
-  </si>
-  <si>
     <t>illustrative gestures</t>
   </si>
   <si>
@@ -295,21 +190,9 @@
     <t>0.34179357021996615</t>
   </si>
   <si>
-    <t>0.2733552044436531</t>
-  </si>
-  <si>
-    <t>0.9167494793398472</t>
-  </si>
-  <si>
     <t>shaking legs</t>
   </si>
   <si>
-    <t>0.20205314461716187</t>
-  </si>
-  <si>
-    <t>0.8482829751618958</t>
-  </si>
-  <si>
     <t>curling legs</t>
   </si>
   <si>
@@ -322,33 +205,15 @@
     <t>0.6181818181818182</t>
   </si>
   <si>
-    <t>0.9074128644631075</t>
-  </si>
-  <si>
     <t>spread legs</t>
   </si>
   <si>
-    <t>0.11387568918767213</t>
-  </si>
-  <si>
-    <t>0.9330854653900487</t>
-  </si>
-  <si>
     <t>closing legs</t>
   </si>
   <si>
-    <t>0.11680497027426104</t>
-  </si>
-  <si>
-    <t>0.9377802606235703</t>
-  </si>
-  <si>
     <t>crossing legs</t>
   </si>
   <si>
-    <t>0.22367652123427972</t>
-  </si>
-  <si>
     <t>stretching feet</t>
   </si>
   <si>
@@ -361,9 +226,6 @@
     <t>0.4403669724770642</t>
   </si>
   <si>
-    <t>0.46704596195354425</t>
-  </si>
-  <si>
     <t>retracting feet</t>
   </si>
   <si>
@@ -373,12 +235,6 @@
     <t>0.3786666666666667</t>
   </si>
   <si>
-    <t>0.32849849308337253</t>
-  </si>
-  <si>
-    <t>0.9556857479846097</t>
-  </si>
-  <si>
     <t>tiptoe</t>
   </si>
   <si>
@@ -391,129 +247,54 @@
     <t>0.2992125984251969</t>
   </si>
   <si>
-    <t>0.3027987820971947</t>
-  </si>
-  <si>
-    <t>0.9199394651788861</t>
-  </si>
-  <si>
     <t>scratching or touching neck</t>
   </si>
   <si>
-    <t>0.1025491761811282</t>
-  </si>
-  <si>
-    <t>0.9511819054475643</t>
-  </si>
-  <si>
     <t>scratching or touching chest</t>
   </si>
   <si>
-    <t>0.1433255038575177</t>
-  </si>
-  <si>
-    <t>0.9507618103137396</t>
-  </si>
-  <si>
     <t>scratching or touching back</t>
   </si>
   <si>
-    <t>0.2629691974315481</t>
-  </si>
-  <si>
     <t>scratching or touching shoulder</t>
   </si>
   <si>
-    <t>0.9715776481149013</t>
-  </si>
-  <si>
     <t>arms akimbo</t>
   </si>
   <si>
-    <t>0.3383922799727443</t>
-  </si>
-  <si>
-    <t>0.9454584349463055</t>
-  </si>
-  <si>
     <t>crossing arms</t>
   </si>
   <si>
-    <t>0.2880017378695525</t>
-  </si>
-  <si>
-    <t>0.9171352856629538</t>
-  </si>
-  <si>
     <t>playing or tidying hair</t>
   </si>
   <si>
-    <t>0.9534054000852991</t>
-  </si>
-  <si>
     <t>scratching or touching hindbrain</t>
   </si>
   <si>
-    <t>0.9638140100973676</t>
-  </si>
-  <si>
     <t>scratching or touching forehead</t>
   </si>
   <si>
-    <t>0.9574551483061738</t>
-  </si>
-  <si>
     <t>scratching or touching face</t>
   </si>
   <si>
-    <t>0.1665772923027137</t>
-  </si>
-  <si>
-    <t>0.9585125981106426</t>
-  </si>
-  <si>
     <t>rubbing eyes</t>
   </si>
   <si>
-    <t>0.9601880501394278</t>
-  </si>
-  <si>
     <t>touching nose</t>
   </si>
   <si>
-    <t>0.22029604751737256</t>
-  </si>
-  <si>
-    <t>0.9623193991053077</t>
-  </si>
-  <si>
     <t>touching ears</t>
   </si>
   <si>
-    <t>0.9724941557273872</t>
-  </si>
-  <si>
     <t>covering face</t>
   </si>
   <si>
-    <t>0.9107718481375359</t>
-  </si>
-  <si>
     <t>covering mouth</t>
   </si>
   <si>
-    <t>0.028653206072326815</t>
-  </si>
-  <si>
-    <t>0.9022619901925606</t>
-  </si>
-  <si>
     <t>pushing glasses</t>
   </si>
   <si>
-    <t>0.9550294541447704</t>
-  </si>
-  <si>
     <t>patting legs</t>
   </si>
   <si>
@@ -526,12 +307,6 @@
     <t>0.4923076923076923</t>
   </si>
   <si>
-    <t>0.4654220583594056</t>
-  </si>
-  <si>
-    <t>0.9381153824592251</t>
-  </si>
-  <si>
     <t>touching legs</t>
   </si>
   <si>
@@ -544,30 +319,12 @@
     <t>0.43223443223443225</t>
   </si>
   <si>
-    <t>0.41228286511986817</t>
-  </si>
-  <si>
-    <t>0.9199542386299085</t>
-  </si>
-  <si>
     <t>scratching legs</t>
   </si>
   <si>
-    <t>0.11843788968228088</t>
-  </si>
-  <si>
-    <t>0.9383945938358499</t>
-  </si>
-  <si>
     <t>scratching feet</t>
   </si>
   <si>
-    <t>0.030288175059974422</t>
-  </si>
-  <si>
-    <t>0.9091104734576758</t>
-  </si>
-  <si>
     <t>body</t>
   </si>
   <si>
@@ -695,12 +452,18 @@
   </si>
   <si>
     <t>0.49492438579441794</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1178,9 +941,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1226,7 +991,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1237,6 +1009,1307 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>classification_report!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>support</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.1399030847680957E-3"/>
+                  <c:y val="-0.30303696412948383"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>classification_report!$F$2:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>classification_report!$G$2:$G$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0.36916701849960598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.192497311916735</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0000">
+                  <c:v>8.3938467103573493E-3</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000">
+                  <c:v>2.2600236227801902E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.431628242743957</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>5.7268484566949503E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>7.8426121578777694E-2</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>9.9431778418725594E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21718854985321601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.356035613865119</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35907221404293799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.38874374254403199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1903223956589998E-2</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0000">
+                  <c:v>4.27232735263098E-2</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0000">
+                  <c:v>9.1401827473178196E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14274661161155699</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.0000">
+                  <c:v>9.4313003652550007E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.220355391234521</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.0000">
+                  <c:v>7.5042279771132606E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.32126225153539001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.154144897623373</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.20397310985488001</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.0000">
+                  <c:v>9.3621254504348494E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.27335520444365302</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.20205314461716101</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.0000">
+                  <c:v>0.56290384076078104</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.11387568918767201</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.116804970274261</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.223676521234279</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.46704596195354398</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.32849849308337198</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.30279878209719402</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.10254917618112799</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.14332550385751699</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26296919743154801</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.0000">
+                  <c:v>8.4670875203108606E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.33839227997274401</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.28800173786955202</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.0000">
+                  <c:v>7.7472914832679804E-2</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.0000">
+                  <c:v>9.8791031300895907E-2</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.0000">
+                  <c:v>5.6871654143629699E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.16657729230271301</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.0000">
+                  <c:v>7.4742054971521393E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.220296047517372</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.0000">
+                  <c:v>9.6242115324105398E-2</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.0000">
+                  <c:v>2.9093097913322598E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.8653206072326801E-2</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.0000">
+                  <c:v>9.4938152100397105E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.46542205835940498</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.412282865119868</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.11843788968228</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.0288175059974401E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3C90-48F5-AE7C-7560C0D160C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1540487360"/>
+        <c:axId val="1540484480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1540487360"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1540484480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1540484480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1540487360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4BC4187-2509-1D08-D39B-C53AB40A241D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC7F4610-B4E3-4681-98E7-41D961D26DB7}" name="Table1" displayName="Table1" ref="A1:I53" totalsRowShown="0">
+  <autoFilter ref="A1:I53" xr:uid="{FC7F4610-B4E3-4681-98E7-41D961D26DB7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I53">
+    <sortCondition ref="A1:A53"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{28A88C19-8954-4105-BA2F-C4D535A3C3C1}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{BA372CBD-D84C-4366-821F-20C961C0DE6F}" name="labels"/>
+    <tableColumn id="3" xr3:uid="{6811865A-DF7D-4755-BC52-94CE9BB108E2}" name="precision"/>
+    <tableColumn id="4" xr3:uid="{1B62FB2F-3300-4D30-BEC9-622C4B001363}" name="recall"/>
+    <tableColumn id="5" xr3:uid="{188F29A7-B902-41EB-A5E9-A61CD4357171}" name="f1-score"/>
+    <tableColumn id="6" xr3:uid="{EB716B73-0876-4550-8E02-3AC6DE071895}" name="support"/>
+    <tableColumn id="7" xr3:uid="{B4FF3F5F-788C-49A9-A5DB-4B131B852E22}" name="AP" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{61CD89B1-3DDB-4912-9232-81ADA3FFF578}" name="AUC" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{DA89C500-FC7E-46B6-A6BF-76E8F1420E90}" name="threshold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D4D5AD79-644F-4B11-AFAF-D176892C5580}" name="Table2" displayName="Table2" ref="L1:T9" totalsRowShown="0">
+  <autoFilter ref="L1:T9" xr:uid="{D4D5AD79-644F-4B11-AFAF-D176892C5580}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{93740D42-67EF-485A-98A5-26B507C64178}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{85815922-1655-4E00-A42A-75D621C4F1CD}" name="labels"/>
+    <tableColumn id="3" xr3:uid="{27B0B2CE-9E5E-4AFE-A648-3F3564125127}" name="precision"/>
+    <tableColumn id="4" xr3:uid="{2C006947-8295-4E86-B2E8-F124E863753E}" name="recall"/>
+    <tableColumn id="5" xr3:uid="{F8E7769B-AAE2-40A3-A455-E5F57A447F85}" name="f1-score"/>
+    <tableColumn id="6" xr3:uid="{A0C9C134-6676-43DF-B6A2-35236618B30C}" name="support"/>
+    <tableColumn id="7" xr3:uid="{566A29BD-E4C6-4CD8-ACAC-2305CE214B85}" name="AP"/>
+    <tableColumn id="8" xr3:uid="{6B4EDEA2-CAB4-4C20-8071-4E62453EA356}" name="AUC"/>
+    <tableColumn id="9" xr3:uid="{F3D01008-D86F-4FB2-89B2-954B77044672}" name="threshold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1556,15 +2629,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C99F784-7684-42DB-9563-F57229EAA69A}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1589,8 +2678,35 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1609,51 +2725,105 @@
       <c r="F2">
         <v>153</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
+      <c r="G2" s="3">
+        <v>0.36916701849960598</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.94128895192655804</v>
       </c>
       <c r="I2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>52</v>
+      </c>
+      <c r="M2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2">
+        <v>467</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F3">
         <v>74</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
+      <c r="G3" s="3">
+        <v>0.192497311916735</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.93752329070725204</v>
       </c>
       <c r="I3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q3">
+        <v>2586</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3">
+        <v>0.90240609693219898</v>
+      </c>
+      <c r="T3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1667,22 +2837,49 @@
       <c r="F4">
         <v>9</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>8.3938467103573493E-3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
+      <c r="H4" s="3">
+        <v>0.90000597692905304</v>
       </c>
       <c r="I4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q4">
+        <v>2321</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1696,51 +2893,102 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>2.2600236227801902E-3</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
+      <c r="H5" s="3">
+        <v>0.74350707504925595</v>
       </c>
       <c r="I5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>55</v>
+      </c>
+      <c r="M5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q5">
+        <v>1229</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0.54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>76</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>28</v>
+      <c r="G6" s="3">
+        <v>0.431628242743957</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.95233307861304795</v>
       </c>
       <c r="I6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6">
+        <v>12189</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1754,22 +3002,46 @@
       <c r="F7">
         <v>168</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>5.7268484566949503E-2</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
+      <c r="H7" s="3">
+        <v>0.67442464711982897</v>
       </c>
       <c r="I7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q7">
+        <v>12189</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1783,22 +3055,46 @@
       <c r="F8">
         <v>121</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>7.8426121578777694E-2</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>32</v>
+      <c r="H8" s="3">
+        <v>0.70329141872017997</v>
       </c>
       <c r="I8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>136</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8">
+        <v>12189</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S8">
+        <v>0.89126864114524695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1812,22 +3108,46 @@
       <c r="F9">
         <v>228</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>9.9431778418725594E-2</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>34</v>
+      <c r="H9" s="3">
+        <v>0.71068675795498404</v>
       </c>
       <c r="I9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>59</v>
+      </c>
+      <c r="M9" t="s">
+        <v>140</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q9">
+        <v>12189</v>
+      </c>
+      <c r="R9">
+        <v>0.68198987335946604</v>
+      </c>
+      <c r="S9">
+        <v>0.94115404814321901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1841,109 +3161,109 @@
       <c r="F10">
         <v>480</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
+      <c r="G10" s="3">
+        <v>0.21718854985321601</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.74723997094921002</v>
       </c>
       <c r="I10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>0.53198127925117</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>641</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="3">
+        <v>0.356035613865119</v>
+      </c>
+      <c r="H11" s="2">
         <v>0.85116294843907003</v>
       </c>
       <c r="I11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>0.4375</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F12">
         <v>595</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>46</v>
+      <c r="G12" s="3">
+        <v>0.35907221404293799</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.85435548693530705</v>
       </c>
       <c r="I12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F13">
         <v>112</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>51</v>
+      <c r="G13" s="3">
+        <v>0.38874374254403199</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.94444761600292204</v>
       </c>
       <c r="I13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1957,22 +3277,22 @@
       <c r="F14">
         <v>56</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>54</v>
+      <c r="G14" s="3">
+        <v>4.1903223956589998E-2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.813620511495737</v>
       </c>
       <c r="I14">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1986,22 +3306,22 @@
       <c r="F15">
         <v>47</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>4.27232735263098E-2</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>56</v>
+      <c r="H15" s="3">
+        <v>0.78732239093776002</v>
       </c>
       <c r="I15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2015,11 +3335,11 @@
       <c r="F16">
         <v>21</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>9.1401827473178196E-2</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>58</v>
+      <c r="H16" s="3">
+        <v>0.90840713643948101</v>
       </c>
       <c r="I16">
         <v>0.5</v>
@@ -2030,7 +3350,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2044,11 +3364,11 @@
       <c r="F17">
         <v>41</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>61</v>
+      <c r="G17" s="3">
+        <v>0.14274661161155699</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.93070003738811002</v>
       </c>
       <c r="I17">
         <v>0.5</v>
@@ -2059,7 +3379,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2073,11 +3393,11 @@
       <c r="F18">
         <v>37</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>9.4313003652550007E-2</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>63</v>
+      <c r="H18" s="3">
+        <v>0.83071943812617799</v>
       </c>
       <c r="I18">
         <v>0.5</v>
@@ -2088,25 +3408,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="F19">
         <v>176</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>69</v>
+      <c r="G19" s="3">
+        <v>0.220355391234521</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.925947319778188</v>
       </c>
       <c r="I19">
         <v>0.5</v>
@@ -2117,7 +3437,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2131,11 +3451,11 @@
       <c r="F20">
         <v>43</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>7.5042279771132606E-2</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>71</v>
+      <c r="H20" s="3">
+        <v>0.88896534073983902</v>
       </c>
       <c r="I20">
         <v>0.5</v>
@@ -2146,25 +3466,25 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F21">
         <v>138</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>77</v>
+      <c r="G21" s="3">
+        <v>0.32126225153539001</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.94155214518291497</v>
       </c>
       <c r="I21">
         <v>0.5</v>
@@ -2175,7 +3495,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2189,11 +3509,11 @@
       <c r="F22">
         <v>73</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>80</v>
+      <c r="G22" s="3">
+        <v>0.154144897623373</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.92953765570295799</v>
       </c>
       <c r="I22">
         <v>0.5</v>
@@ -2204,10 +3524,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>1.6949152542372801E-2</v>
@@ -2218,11 +3538,11 @@
       <c r="F23">
         <v>177</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>84</v>
+      <c r="G23" s="3">
+        <v>0.20397310985488001</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.86227390423786199</v>
       </c>
       <c r="I23">
         <v>0.5</v>
@@ -2233,7 +3553,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2247,11 +3567,11 @@
       <c r="F24">
         <v>186</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>9.3621254504348494E-2</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>86</v>
+      <c r="H24" s="3">
+        <v>0.79083333333333306</v>
       </c>
       <c r="I24">
         <v>0.5</v>
@@ -2262,25 +3582,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>197</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>92</v>
+      <c r="G25" s="3">
+        <v>0.27335520444365302</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.91674947933984696</v>
       </c>
       <c r="I25">
         <v>0.5</v>
@@ -2291,7 +3611,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2305,11 +3625,11 @@
       <c r="F26">
         <v>119</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>95</v>
+      <c r="G26" s="3">
+        <v>0.20205314461716101</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.84828297516189499</v>
       </c>
       <c r="I26">
         <v>0.5</v>
@@ -2320,25 +3640,25 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="F27">
         <v>33</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>0.56290384076078104</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>100</v>
+      <c r="H27" s="3">
+        <v>0.90741286446310698</v>
       </c>
       <c r="I27">
         <v>0.5</v>
@@ -2349,7 +3669,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2363,11 +3683,11 @@
       <c r="F28">
         <v>46</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>103</v>
+      <c r="G28" s="3">
+        <v>0.11387568918767201</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.933085465390048</v>
       </c>
       <c r="I28">
         <v>0.5</v>
@@ -2378,7 +3698,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2392,11 +3712,11 @@
       <c r="F29">
         <v>48</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>106</v>
+      <c r="G29" s="3">
+        <v>0.116804970274261</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.93778026062357001</v>
       </c>
       <c r="I29">
         <v>0.5</v>
@@ -2407,7 +3727,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2421,10 +3741,10 @@
       <c r="F30">
         <v>30</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H30">
+      <c r="G30" s="3">
+        <v>0.223676521234279</v>
+      </c>
+      <c r="H30" s="2">
         <v>0.94640328773698101</v>
       </c>
       <c r="I30">
@@ -2436,24 +3756,24 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="F31">
         <v>115</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H31">
+      <c r="G31" s="3">
+        <v>0.46704596195354398</v>
+      </c>
+      <c r="H31" s="2">
         <v>0.96894375879141403</v>
       </c>
       <c r="I31">
@@ -2465,25 +3785,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="D32">
         <v>0.5546875</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="F32">
         <v>128</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>118</v>
+      <c r="G32" s="3">
+        <v>0.32849849308337198</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.95568574798460904</v>
       </c>
       <c r="I32">
         <v>0.5</v>
@@ -2494,25 +3814,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F33">
         <v>198</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>124</v>
+      <c r="G33" s="3">
+        <v>0.30279878209719402</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.91993946517888603</v>
       </c>
       <c r="I33">
         <v>0.5</v>
@@ -2523,7 +3843,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2537,11 +3857,11 @@
       <c r="F34">
         <v>30</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>127</v>
+      <c r="G34" s="3">
+        <v>0.10254917618112799</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.95118190544756398</v>
       </c>
       <c r="I34">
         <v>0.5</v>
@@ -2552,7 +3872,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2566,11 +3886,11 @@
       <c r="F35">
         <v>40</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>130</v>
+      <c r="G35" s="3">
+        <v>0.14332550385751699</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.95076181031373896</v>
       </c>
       <c r="I35">
         <v>0.5</v>
@@ -2581,7 +3901,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2595,10 +3915,10 @@
       <c r="F36">
         <v>25</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H36">
+      <c r="G36" s="3">
+        <v>0.26296919743154801</v>
+      </c>
+      <c r="H36" s="2">
         <v>0.95888509260924304</v>
       </c>
       <c r="I36">
@@ -2610,7 +3930,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2624,11 +3944,11 @@
       <c r="F37">
         <v>16</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2">
         <v>8.4670875203108606E-2</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>134</v>
+      <c r="H37" s="3">
+        <v>0.97157764811490099</v>
       </c>
       <c r="I37">
         <v>0.5</v>
@@ -2639,7 +3959,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2653,11 +3973,11 @@
       <c r="F38">
         <v>21</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>137</v>
+      <c r="G38" s="3">
+        <v>0.33839227997274401</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.94545843494630499</v>
       </c>
       <c r="I38">
         <v>0.5</v>
@@ -2668,7 +3988,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2682,11 +4002,11 @@
       <c r="F39">
         <v>20</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>140</v>
+      <c r="G39" s="3">
+        <v>0.28800173786955202</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.91713528566295299</v>
       </c>
       <c r="I39">
         <v>0.5</v>
@@ -2697,7 +4017,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2711,11 +4031,11 @@
       <c r="F40">
         <v>44</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <v>7.7472914832679804E-2</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>142</v>
+      <c r="H40" s="3">
+        <v>0.95340540008529895</v>
       </c>
       <c r="I40">
         <v>0.5</v>
@@ -2726,7 +4046,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2740,11 +4060,11 @@
       <c r="F41">
         <v>40</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>9.8791031300895907E-2</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>144</v>
+      <c r="H41" s="3">
+        <v>0.963814010097367</v>
       </c>
       <c r="I41">
         <v>0.5</v>
@@ -2755,7 +4075,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2769,11 +4089,11 @@
       <c r="F42">
         <v>28</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>5.6871654143629699E-2</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>146</v>
+      <c r="H42" s="3">
+        <v>0.95745514830617295</v>
       </c>
       <c r="I42">
         <v>0.5</v>
@@ -2784,7 +4104,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2798,11 +4118,11 @@
       <c r="F43">
         <v>63</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>149</v>
+      <c r="G43" s="3">
+        <v>0.16657729230271301</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0.95851259811064204</v>
       </c>
       <c r="I43">
         <v>0.5</v>
@@ -2813,7 +4133,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>85</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2827,11 +4147,11 @@
       <c r="F44">
         <v>33</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="2">
         <v>7.4742054971521393E-2</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>151</v>
+      <c r="H44" s="3">
+        <v>0.96018805013942699</v>
       </c>
       <c r="I44">
         <v>0.5</v>
@@ -2842,7 +4162,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2856,11 +4176,11 @@
       <c r="F45">
         <v>72</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>154</v>
+      <c r="G45" s="3">
+        <v>0.220296047517372</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0.96231939910530695</v>
       </c>
       <c r="I45">
         <v>0.5</v>
@@ -2871,7 +4191,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2885,11 +4205,11 @@
       <c r="F46">
         <v>25</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>9.6242115324105398E-2</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>156</v>
+      <c r="H46" s="3">
+        <v>0.97249415572738696</v>
       </c>
       <c r="I46">
         <v>0.5</v>
@@ -2900,7 +4220,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2914,11 +4234,11 @@
       <c r="F47">
         <v>2</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>2.9093097913322598E-3</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>158</v>
+      <c r="H47" s="3">
+        <v>0.91077184813753498</v>
       </c>
       <c r="I47">
         <v>0.5</v>
@@ -2929,7 +4249,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2943,11 +4263,11 @@
       <c r="F48">
         <v>12</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>161</v>
+      <c r="G48" s="3">
+        <v>2.8653206072326801E-2</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0.90226199019256004</v>
       </c>
       <c r="I48">
         <v>0.5</v>
@@ -2958,7 +4278,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2972,11 +4292,11 @@
       <c r="F49">
         <v>34</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>9.4938152100397105E-2</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>163</v>
+      <c r="H49" s="3">
+        <v>0.95502945414477003</v>
       </c>
       <c r="I49">
         <v>0.5</v>
@@ -2987,25 +4307,25 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
       <c r="F50">
         <v>209</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>169</v>
+      <c r="G50" s="3">
+        <v>0.46542205835940498</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0.93811538245922499</v>
       </c>
       <c r="I50">
         <v>0.5</v>
@@ -3016,25 +4336,25 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="F51">
         <v>248</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>175</v>
+      <c r="G51" s="3">
+        <v>0.412282865119868</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0.91995423862990799</v>
       </c>
       <c r="I51">
         <v>0.5</v>
@@ -3045,7 +4365,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>99</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -3059,11 +4379,11 @@
       <c r="F52">
         <v>45</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>178</v>
+      <c r="G52" s="3">
+        <v>0.11843788968228</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0.938394593835849</v>
       </c>
       <c r="I52">
         <v>0.5</v>
@@ -3074,7 +4394,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>100</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -3088,237 +4408,22 @@
       <c r="F53">
         <v>10</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>181</v>
+      <c r="G53" s="3">
+        <v>3.0288175059974401E-2</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0.90911047345767504</v>
       </c>
       <c r="I53">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>182</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F54">
-        <v>467</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I54">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>188</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F55">
-        <v>2586</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H55">
-        <v>0.90240609693219898</v>
-      </c>
-      <c r="I55">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>193</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F56">
-        <v>2321</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="I56">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>199</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F57">
-        <v>1229</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I57">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>205</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F58">
-        <v>12189</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>211</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F59">
-        <v>12189</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>217</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F60">
-        <v>12189</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H60">
-        <v>0.89126864114524695</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>221</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F61">
-        <v>12189</v>
-      </c>
-      <c r="G61">
-        <v>0.68198987335946604</v>
-      </c>
-      <c r="H61">
-        <v>0.94115404814321901</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>